<commit_message>
Changed LR2 and LR3
</commit_message>
<xml_diff>
--- a/LR3/table_1_59.xlsx
+++ b/LR3/table_1_59.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2daf2d85f4952eb5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="11_924874E5C5FBB6926123EA198B3E8C185103838B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAD2555D-22DB-496D-AA3C-4242E3BD6F97}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22B68D9-2357-48F8-A62E-2CE573D705DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -68,114 +66,6 @@
     <t>Итого</t>
   </si>
   <si>
-    <t>Алишеров</t>
-  </si>
-  <si>
-    <t>Аллаярова</t>
-  </si>
-  <si>
-    <t>Антипов</t>
-  </si>
-  <si>
-    <t>Арсланов</t>
-  </si>
-  <si>
-    <t>Гусаков</t>
-  </si>
-  <si>
-    <t>Дедюхин</t>
-  </si>
-  <si>
-    <t>Иванова</t>
-  </si>
-  <si>
-    <t>Камалов</t>
-  </si>
-  <si>
-    <t>Любенко</t>
-  </si>
-  <si>
-    <t>Максутов</t>
-  </si>
-  <si>
-    <t>Никифорович</t>
-  </si>
-  <si>
-    <t>Овчинников</t>
-  </si>
-  <si>
-    <t>Романова</t>
-  </si>
-  <si>
-    <t>Симоненко</t>
-  </si>
-  <si>
-    <t>Стариков</t>
-  </si>
-  <si>
-    <t>Сулейманов</t>
-  </si>
-  <si>
-    <t>Тураев</t>
-  </si>
-  <si>
-    <t>Хакимджанов</t>
-  </si>
-  <si>
-    <t>Хасанов</t>
-  </si>
-  <si>
-    <t>Чарыев</t>
-  </si>
-  <si>
-    <t>Юсупова</t>
-  </si>
-  <si>
-    <t>Куропаткин 1</t>
-  </si>
-  <si>
-    <t>Куропаткин 2</t>
-  </si>
-  <si>
-    <t>Куропаткин 3</t>
-  </si>
-  <si>
-    <t>Куропаткин 4</t>
-  </si>
-  <si>
-    <t>Куропаткин 5</t>
-  </si>
-  <si>
-    <t>Куропаткин 6</t>
-  </si>
-  <si>
-    <t>Куропаткин 7</t>
-  </si>
-  <si>
-    <t>Куропаткин 8</t>
-  </si>
-  <si>
-    <t>Куропаткин 9</t>
-  </si>
-  <si>
-    <t>Куропаткин 10</t>
-  </si>
-  <si>
-    <t>Куропаткин 11</t>
-  </si>
-  <si>
-    <t>Куропаткин 12</t>
-  </si>
-  <si>
-    <t>Куропаткин 13</t>
-  </si>
-  <si>
-    <t>Куропаткин 14</t>
-  </si>
-  <si>
-    <t>Куропаткин 15</t>
-  </si>
-  <si>
     <t>Общая сумма графы “Итого”</t>
   </si>
   <si>
@@ -186,13 +76,121 @@
   </si>
   <si>
     <t>Максимальная сумма к оплате</t>
+  </si>
+  <si>
+    <t>Дедю́хин</t>
+  </si>
+  <si>
+    <t>Алише́ров</t>
+  </si>
+  <si>
+    <t>Аллая́рова</t>
+  </si>
+  <si>
+    <t>Анти́пов</t>
+  </si>
+  <si>
+    <t>Арсла́нов</t>
+  </si>
+  <si>
+    <t>Гусако́в</t>
+  </si>
+  <si>
+    <t>Ивано́ва</t>
+  </si>
+  <si>
+    <t>Кама́лов</t>
+  </si>
+  <si>
+    <t>Любе́нко</t>
+  </si>
+  <si>
+    <t>Максу́тов</t>
+  </si>
+  <si>
+    <t>Никифоро́вич</t>
+  </si>
+  <si>
+    <t>Овчи́нников</t>
+  </si>
+  <si>
+    <t>Рома́нова</t>
+  </si>
+  <si>
+    <t>Симоне́нко</t>
+  </si>
+  <si>
+    <t>Ста́риков</t>
+  </si>
+  <si>
+    <t>Сулейма́нов</t>
+  </si>
+  <si>
+    <t>Тура́ев</t>
+  </si>
+  <si>
+    <t>Хакимджа́нов</t>
+  </si>
+  <si>
+    <t>Хаса́нов</t>
+  </si>
+  <si>
+    <t>Чары́ев</t>
+  </si>
+  <si>
+    <t>Юсу́пова</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 1</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 2</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 3</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 4</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 5</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 6</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 7</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 8</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 9</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 10</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 11</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 12</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 13</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 14</t>
+  </si>
+  <si>
+    <t>Куропа́ткин 15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,19 +199,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF282C34"/>
-      <name val="Times New Roman"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -236,25 +231,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,35 +555,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="2"/>
-    <col min="6" max="6" width="14.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="13" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="1"/>
+    <col min="6" max="6" width="14.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>59</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -631,12 +613,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>11</v>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="1">
         <v>70</v>
@@ -649,10 +631,10 @@
         <f>C3*D3</f>
         <v>4543</v>
       </c>
-      <c r="F3" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="F3" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G3" s="2">
         <v>44805</v>
       </c>
       <c r="H3" s="1">
@@ -671,12 +653,12 @@
         <v>4543</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>12</v>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C4" s="1">
         <v>69.5</v>
@@ -689,10 +671,10 @@
         <f t="shared" ref="E4:E38" si="1">C4*D4</f>
         <v>4510.55</v>
       </c>
-      <c r="F4" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G4" s="5">
+      <c r="F4" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G4" s="2">
         <v>44806</v>
       </c>
       <c r="H4" s="1">
@@ -711,12 +693,12 @@
         <v>4510.55</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>13</v>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C5" s="1">
         <v>69</v>
@@ -729,10 +711,10 @@
         <f t="shared" si="1"/>
         <v>4478.1000000000004</v>
       </c>
-      <c r="F5" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G5" s="5">
+      <c r="F5" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G5" s="2">
         <v>44807</v>
       </c>
       <c r="H5" s="1">
@@ -751,12 +733,12 @@
         <v>4478.1000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>14</v>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C6" s="1">
         <v>68.5</v>
@@ -769,10 +751,10 @@
         <f t="shared" si="1"/>
         <v>4445.6500000000005</v>
       </c>
-      <c r="F6" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G6" s="5">
+      <c r="F6" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G6" s="2">
         <v>44808</v>
       </c>
       <c r="H6" s="1">
@@ -791,12 +773,12 @@
         <v>4445.6500000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>15</v>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C7" s="1">
         <v>68</v>
@@ -809,10 +791,10 @@
         <f t="shared" si="1"/>
         <v>4413.2000000000007</v>
       </c>
-      <c r="F7" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G7" s="5">
+      <c r="F7" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G7" s="2">
         <v>44809</v>
       </c>
       <c r="H7" s="1">
@@ -831,12 +813,12 @@
         <v>4413.2000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>16</v>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>67.5</v>
@@ -849,10 +831,10 @@
         <f t="shared" si="1"/>
         <v>4380.75</v>
       </c>
-      <c r="F8" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="F8" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G8" s="2">
         <v>44810</v>
       </c>
       <c r="H8" s="1">
@@ -871,12 +853,12 @@
         <v>4380.75</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>17</v>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="1">
         <v>67</v>
@@ -889,10 +871,10 @@
         <f t="shared" si="1"/>
         <v>4348.3</v>
       </c>
-      <c r="F9" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G9" s="5">
+      <c r="F9" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G9" s="2">
         <v>44811</v>
       </c>
       <c r="H9" s="1">
@@ -911,12 +893,12 @@
         <v>4348.3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>18</v>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C10" s="1">
         <v>66.5</v>
@@ -929,10 +911,10 @@
         <f t="shared" si="1"/>
         <v>4315.8500000000004</v>
       </c>
-      <c r="F10" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G10" s="5">
+      <c r="F10" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G10" s="2">
         <v>44812</v>
       </c>
       <c r="H10" s="1">
@@ -951,12 +933,12 @@
         <v>4315.8500000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>19</v>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C11" s="1">
         <v>66</v>
@@ -969,10 +951,10 @@
         <f t="shared" si="1"/>
         <v>4283.4000000000005</v>
       </c>
-      <c r="F11" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G11" s="5">
+      <c r="F11" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G11" s="2">
         <v>44813</v>
       </c>
       <c r="H11" s="1">
@@ -991,12 +973,12 @@
         <v>4283.4000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>20</v>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C12" s="1">
         <v>65.5</v>
@@ -1009,10 +991,10 @@
         <f t="shared" si="1"/>
         <v>4250.9500000000007</v>
       </c>
-      <c r="F12" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G12" s="5">
+      <c r="F12" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G12" s="2">
         <v>44814</v>
       </c>
       <c r="H12" s="1">
@@ -1031,12 +1013,12 @@
         <v>4260.9500000000007</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>21</v>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C13" s="1">
         <v>65</v>
@@ -1049,10 +1031,10 @@
         <f t="shared" si="1"/>
         <v>4218.5</v>
       </c>
-      <c r="F13" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G13" s="5">
+      <c r="F13" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G13" s="2">
         <v>44815</v>
       </c>
       <c r="H13" s="1">
@@ -1071,12 +1053,12 @@
         <v>4238.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>22</v>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C14" s="1">
         <v>64.5</v>
@@ -1089,10 +1071,10 @@
         <f t="shared" si="1"/>
         <v>4186.05</v>
       </c>
-      <c r="F14" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G14" s="5">
+      <c r="F14" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G14" s="2">
         <v>44816</v>
       </c>
       <c r="H14" s="1">
@@ -1111,12 +1093,12 @@
         <v>4216.05</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>23</v>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C15" s="1">
         <v>64</v>
@@ -1129,10 +1111,10 @@
         <f t="shared" si="1"/>
         <v>4153.6000000000004</v>
       </c>
-      <c r="F15" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G15" s="5">
+      <c r="F15" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G15" s="2">
         <v>44817</v>
       </c>
       <c r="H15" s="1">
@@ -1151,12 +1133,12 @@
         <v>4193.6000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>24</v>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C16" s="1">
         <v>63.5</v>
@@ -1169,10 +1151,10 @@
         <f t="shared" si="1"/>
         <v>4121.1500000000005</v>
       </c>
-      <c r="F16" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G16" s="5">
+      <c r="F16" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G16" s="2">
         <v>44818</v>
       </c>
       <c r="H16" s="1">
@@ -1191,12 +1173,12 @@
         <v>4171.1500000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>25</v>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C17" s="1">
         <v>63</v>
@@ -1209,10 +1191,10 @@
         <f t="shared" si="1"/>
         <v>4088.7000000000003</v>
       </c>
-      <c r="F17" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G17" s="5">
+      <c r="F17" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G17" s="2">
         <v>44819</v>
       </c>
       <c r="H17" s="1">
@@ -1231,12 +1213,12 @@
         <v>4148.7000000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>26</v>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C18" s="1">
         <v>62.5</v>
@@ -1249,10 +1231,10 @@
         <f t="shared" si="1"/>
         <v>4056.2500000000005</v>
       </c>
-      <c r="F18" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G18" s="5">
+      <c r="F18" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G18" s="2">
         <v>44820</v>
       </c>
       <c r="H18" s="1">
@@ -1271,12 +1253,12 @@
         <v>4126.25</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>27</v>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C19" s="1">
         <v>62</v>
@@ -1289,10 +1271,10 @@
         <f t="shared" si="1"/>
         <v>4023.8</v>
       </c>
-      <c r="F19" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G19" s="5">
+      <c r="F19" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G19" s="2">
         <v>44821</v>
       </c>
       <c r="H19" s="1">
@@ -1311,12 +1293,12 @@
         <v>4103.8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>28</v>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C20" s="1">
         <v>61.5</v>
@@ -1329,10 +1311,10 @@
         <f t="shared" si="1"/>
         <v>3991.3500000000004</v>
       </c>
-      <c r="F20" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G20" s="5">
+      <c r="F20" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G20" s="2">
         <v>44822</v>
       </c>
       <c r="H20" s="1">
@@ -1351,12 +1333,12 @@
         <v>4081.3500000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>29</v>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C21" s="1">
         <v>61</v>
@@ -1369,10 +1351,10 @@
         <f t="shared" si="1"/>
         <v>3958.9000000000005</v>
       </c>
-      <c r="F21" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G21" s="5">
+      <c r="F21" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G21" s="2">
         <v>44823</v>
       </c>
       <c r="H21" s="1">
@@ -1391,12 +1373,12 @@
         <v>4058.9000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>30</v>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C22" s="1">
         <v>60.5</v>
@@ -1409,10 +1391,10 @@
         <f t="shared" si="1"/>
         <v>3926.4500000000003</v>
       </c>
-      <c r="F22" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G22" s="5">
+      <c r="F22" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G22" s="2">
         <v>44824</v>
       </c>
       <c r="H22" s="1">
@@ -1431,12 +1413,12 @@
         <v>4036.4500000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>31</v>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C23" s="1">
         <v>60</v>
@@ -1449,10 +1431,10 @@
         <f t="shared" si="1"/>
         <v>3894.0000000000005</v>
       </c>
-      <c r="F23" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G23" s="5">
+      <c r="F23" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G23" s="2">
         <v>44825</v>
       </c>
       <c r="H23" s="1">
@@ -1471,12 +1453,12 @@
         <v>4014.0000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1">
         <v>59.5</v>
@@ -1489,10 +1471,10 @@
         <f t="shared" si="1"/>
         <v>3861.55</v>
       </c>
-      <c r="F24" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G24" s="5">
+      <c r="F24" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G24" s="2">
         <v>44826</v>
       </c>
       <c r="H24" s="1">
@@ -1511,12 +1493,12 @@
         <v>3991.55</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C25" s="1">
         <v>59</v>
@@ -1529,10 +1511,10 @@
         <f t="shared" si="1"/>
         <v>3829.1000000000004</v>
       </c>
-      <c r="F25" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G25" s="5">
+      <c r="F25" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G25" s="2">
         <v>44827</v>
       </c>
       <c r="H25" s="1">
@@ -1551,12 +1533,12 @@
         <v>3969.1000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1">
         <v>58.5</v>
@@ -1569,10 +1551,10 @@
         <f t="shared" si="1"/>
         <v>3796.6500000000005</v>
       </c>
-      <c r="F26" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G26" s="5">
+      <c r="F26" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G26" s="2">
         <v>44828</v>
       </c>
       <c r="H26" s="1">
@@ -1591,12 +1573,12 @@
         <v>3946.6500000000005</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C27" s="1">
         <v>58</v>
@@ -1609,10 +1591,10 @@
         <f t="shared" si="1"/>
         <v>3764.2000000000003</v>
       </c>
-      <c r="F27" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G27" s="5">
+      <c r="F27" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G27" s="2">
         <v>44829</v>
       </c>
       <c r="H27" s="1">
@@ -1631,12 +1613,12 @@
         <v>3924.2000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C28" s="1">
         <v>57.5</v>
@@ -1649,10 +1631,10 @@
         <f t="shared" si="1"/>
         <v>3731.7500000000005</v>
       </c>
-      <c r="F28" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G28" s="5">
+      <c r="F28" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G28" s="2">
         <v>44830</v>
       </c>
       <c r="H28" s="1">
@@ -1671,12 +1653,12 @@
         <v>3901.7500000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C29" s="1">
         <v>57</v>
@@ -1689,10 +1671,10 @@
         <f t="shared" si="1"/>
         <v>3699.3</v>
       </c>
-      <c r="F29" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G29" s="5">
+      <c r="F29" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G29" s="2">
         <v>44831</v>
       </c>
       <c r="H29" s="1">
@@ -1711,12 +1693,12 @@
         <v>3879.3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C30" s="1">
         <v>56.5</v>
@@ -1729,10 +1711,10 @@
         <f t="shared" si="1"/>
         <v>3666.8500000000004</v>
       </c>
-      <c r="F30" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G30" s="5">
+      <c r="F30" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G30" s="2">
         <v>44832</v>
       </c>
       <c r="H30" s="1">
@@ -1751,12 +1733,12 @@
         <v>3856.8500000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C31" s="1">
         <v>56</v>
@@ -1769,10 +1751,10 @@
         <f t="shared" si="1"/>
         <v>3634.4000000000005</v>
       </c>
-      <c r="F31" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G31" s="5">
+      <c r="F31" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G31" s="2">
         <v>44833</v>
       </c>
       <c r="H31" s="1">
@@ -1791,12 +1773,12 @@
         <v>3834.4000000000005</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C32" s="1">
         <v>55.5</v>
@@ -1809,10 +1791,10 @@
         <f t="shared" si="1"/>
         <v>3601.9500000000003</v>
       </c>
-      <c r="F32" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G32" s="5">
+      <c r="F32" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G32" s="2">
         <v>44834</v>
       </c>
       <c r="H32" s="1">
@@ -1831,12 +1813,12 @@
         <v>3811.9500000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C33" s="1">
         <v>55</v>
@@ -1849,10 +1831,10 @@
         <f t="shared" si="1"/>
         <v>3569.5000000000005</v>
       </c>
-      <c r="F33" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G33" s="5">
+      <c r="F33" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G33" s="2">
         <v>44835</v>
       </c>
       <c r="H33" s="1">
@@ -1871,12 +1853,12 @@
         <v>3789.5000000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C34" s="1">
         <v>54.5</v>
@@ -1889,10 +1871,10 @@
         <f t="shared" si="1"/>
         <v>3537.05</v>
       </c>
-      <c r="F34" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G34" s="5">
+      <c r="F34" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G34" s="2">
         <v>44836</v>
       </c>
       <c r="H34" s="1">
@@ -1911,12 +1893,12 @@
         <v>3767.05</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C35" s="1">
         <v>54</v>
@@ -1929,10 +1911,10 @@
         <f t="shared" si="1"/>
         <v>1752.3000000000002</v>
       </c>
-      <c r="F35" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G35" s="5">
+      <c r="F35" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G35" s="2">
         <v>44837</v>
       </c>
       <c r="H35" s="1">
@@ -1951,12 +1933,12 @@
         <v>1992.3000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1">
         <v>53.5</v>
@@ -1969,10 +1951,10 @@
         <f t="shared" si="1"/>
         <v>1736.075</v>
       </c>
-      <c r="F36" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G36" s="5">
+      <c r="F36" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G36" s="2">
         <v>44838</v>
       </c>
       <c r="H36" s="1">
@@ -1991,12 +1973,12 @@
         <v>1986.075</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C37" s="1">
         <v>53</v>
@@ -2009,10 +1991,10 @@
         <f t="shared" si="1"/>
         <v>1719.8500000000001</v>
       </c>
-      <c r="F37" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G37" s="5">
+      <c r="F37" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G37" s="2">
         <v>44839</v>
       </c>
       <c r="H37" s="1">
@@ -2031,12 +2013,12 @@
         <v>1979.8500000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C38" s="1">
         <v>52.5</v>
@@ -2049,10 +2031,10 @@
         <f t="shared" si="1"/>
         <v>1703.6250000000002</v>
       </c>
-      <c r="F38" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G38" s="5">
+      <c r="F38" s="2">
+        <v>44813</v>
+      </c>
+      <c r="G38" s="2">
         <v>44840</v>
       </c>
       <c r="H38" s="1">
@@ -2071,36 +2053,36 @@
         <v>1973.6250000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B40" s="4" t="s">
-        <v>47</v>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C40" s="1">
         <f>INT(SUM(K3:K38))</f>
         <v>139972</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B41" s="4" t="s">
-        <v>48</v>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B41" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C41" s="1">
         <f>AVERAGE(C3:C38)</f>
         <v>61.25</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B42" s="4" t="s">
-        <v>49</v>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B42" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C42" s="1">
         <f>MAX(H3:H38)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B43" s="4" t="s">
-        <v>50</v>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B43" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C43" s="1">
         <f>MAX(K3:K38)</f>
@@ -2108,6 +2090,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>